<commit_message>
Update Allure test reports by replacing old results and attachments with new data and modifying report metadata.
</commit_message>
<xml_diff>
--- a/test-data/loginpage1data.xlsx
+++ b/test-data/loginpage1data.xlsx
@@ -451,10 +451,10 @@
         <v>Fail</v>
       </c>
       <c r="G2" t="str">
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>Fail</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="str">
         <v>Login was unsuccessful</v>
@@ -506,7 +506,7 @@
         <v>Fail</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <v>Login was unsuccessful</v>
@@ -535,7 +535,7 @@
         <v>Fail</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="str">
         <v>Login was unsuccessful</v>
@@ -561,7 +561,7 @@
         <v>Fail</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="str">
         <v>Please enter your email</v>
@@ -587,7 +587,7 @@
         <v>Fail</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="str">
         <v>Login was unsuccessful</v>
@@ -610,7 +610,7 @@
         <v>Fail</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <v>Please enter your email</v>
@@ -639,7 +639,7 @@
         <v>Fail</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -665,7 +665,7 @@
         <v>Fail</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="str">
         <v>Login was unsuccessful</v>
@@ -694,7 +694,7 @@
         <v>Fail</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -717,10 +717,10 @@
         <v>Pass</v>
       </c>
       <c r="G12" t="str">
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -743,10 +743,10 @@
         <v>Pass</v>
       </c>
       <c r="G13" t="str">
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -769,10 +769,10 @@
         <v>Pass</v>
       </c>
       <c r="G14" t="str">
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -824,7 +824,7 @@
         <v>Fail</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -850,7 +850,7 @@
         <v>Fail</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -876,7 +876,7 @@
         <v>Fail</v>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -902,7 +902,7 @@
         <v>Fail</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="str">
         <v>Login was unsuccessful</v>
@@ -931,7 +931,7 @@
         <v>Fail</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="str">
         <v>Login was unsuccessful</v>
@@ -960,7 +960,7 @@
         <v>Fail</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="str">
         <v>Login was unsuccessful</v>
@@ -989,7 +989,7 @@
         <v>Fail</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1015,7 +1015,7 @@
         <v>Fail</v>
       </c>
       <c r="H23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1041,7 +1041,7 @@
         <v>Fail</v>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1067,7 +1067,7 @@
         <v>Fail</v>
       </c>
       <c r="H25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="str">
         <v>Login was unsuccessful</v>
@@ -1096,7 +1096,7 @@
         <v>Fail</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="str">
         <v>Login was unsuccessful</v>
@@ -1125,7 +1125,7 @@
         <v>Fail</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="str">
         <v>Login was unsuccessful</v>
@@ -1154,7 +1154,7 @@
         <v>Fail</v>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="str">
         <v>Login was unsuccessful</v>
@@ -1183,7 +1183,7 @@
         <v>Fail</v>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1209,7 +1209,7 @@
         <v>Fail</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" xml:space="preserve">
@@ -1236,7 +1236,7 @@
         <v>Fail</v>
       </c>
       <c r="H31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1262,7 +1262,7 @@
         <v>Fail</v>
       </c>
       <c r="H32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="str">
         <v>Login was unsuccessful</v>
@@ -1292,7 +1292,7 @@
         <v>Fail</v>
       </c>
       <c r="H33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="str">
         <v>Login was unsuccessful</v>
@@ -1321,7 +1321,7 @@
         <v>Fail</v>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="str">
         <v>Login was unsuccessful</v>
@@ -1350,7 +1350,7 @@
         <v>Fail</v>
       </c>
       <c r="H35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="str">
         <v>Login was unsuccessful</v>
@@ -1379,7 +1379,7 @@
         <v>Fail</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="str">
         <v>Login was unsuccessful</v>
@@ -1408,7 +1408,7 @@
         <v>Fail</v>
       </c>
       <c r="H37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1434,7 +1434,7 @@
         <v>Fail</v>
       </c>
       <c r="H38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1460,7 +1460,7 @@
         <v>Fail</v>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1486,7 +1486,7 @@
         <v>Fail</v>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1512,7 +1512,7 @@
         <v>Fail</v>
       </c>
       <c r="H41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="str">
         <v>Login was unsuccessful</v>
@@ -1541,7 +1541,7 @@
         <v>Fail</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="str">
         <v>Login was unsuccessful</v>
@@ -1570,7 +1570,7 @@
         <v>Pass</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1596,7 +1596,7 @@
         <v>Pass</v>
       </c>
       <c r="H44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1622,7 +1622,7 @@
         <v>Fail</v>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1648,7 +1648,7 @@
         <v>Fail</v>
       </c>
       <c r="H46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1674,7 +1674,7 @@
         <v>Fail</v>
       </c>
       <c r="H47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1700,7 +1700,7 @@
         <v>Fail</v>
       </c>
       <c r="H48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1726,7 +1726,7 @@
         <v>Fail</v>
       </c>
       <c r="H49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="str">
         <v>Login was unsuccessful</v>
@@ -1755,7 +1755,7 @@
         <v>Fail</v>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="str">
         <v>Sorry, you have been blocked</v>
@@ -1784,7 +1784,7 @@
         <v>Fail</v>
       </c>
       <c r="H51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="str">
         <v>Login was unsuccessful</v>
@@ -1813,7 +1813,7 @@
         <v>Fail</v>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="str">
         <v>Login was unsuccessful</v>
@@ -1842,7 +1842,7 @@
         <v>Fail</v>
       </c>
       <c r="H53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1868,7 +1868,7 @@
         <v>Fail</v>
       </c>
       <c r="H54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1894,7 +1894,7 @@
         <v>Fail</v>
       </c>
       <c r="H55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1920,7 +1920,7 @@
         <v>Fail</v>
       </c>
       <c r="H56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1946,7 +1946,7 @@
         <v>Fail</v>
       </c>
       <c r="H57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="str">
         <v>Login was unsuccessful</v>

</xml_diff>

<commit_message>
Modified Jenkinsfile and test data, and updated Allure test reports.
</commit_message>
<xml_diff>
--- a/test-data/loginpage1data.xlsx
+++ b/test-data/loginpage1data.xlsx
@@ -456,6 +456,9 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -502,6 +505,9 @@
       <c r="E4" t="b">
         <v>0</v>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
       <c r="G4" t="str">
         <v>Fail</v>
       </c>
@@ -548,6 +554,9 @@
       <c r="B6" t="str">
         <v>Negative - Empty Email</v>
       </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
       <c r="D6" t="str">
         <v>admin</v>
       </c>
@@ -577,6 +586,9 @@
       <c r="C7" t="str">
         <v>admin@yourstore.com</v>
       </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
@@ -600,6 +612,12 @@
       <c r="B8" t="str">
         <v>Negative - Both Empty</v>
       </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
@@ -641,6 +659,9 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -696,6 +717,9 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -722,6 +746,9 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -748,6 +775,9 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -774,6 +804,9 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -798,7 +831,10 @@
         <v>Fail</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I15" t="str">
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -826,6 +862,9 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -852,6 +891,9 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -878,6 +920,9 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -991,6 +1036,9 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
+      <c r="I22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1017,6 +1065,9 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
+      <c r="I23" t="str">
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1043,6 +1094,9 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
+      <c r="I24" t="str">
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1185,6 +1239,9 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
+      <c r="I29" t="str">
+        <v/>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1211,6 +1268,9 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
+      <c r="I30" t="str">
+        <v/>
+      </c>
     </row>
     <row r="31" xml:space="preserve">
       <c r="A31" t="str">
@@ -1238,6 +1298,9 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
+      <c r="I31" t="str">
+        <v/>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1410,6 +1473,9 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
+      <c r="I37" t="str">
+        <v/>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1436,6 +1502,9 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1462,6 +1531,9 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
+      <c r="I39" t="str">
+        <v/>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1488,6 +1560,9 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
+      <c r="I40" t="str">
+        <v/>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1567,10 +1642,13 @@
         <v>Pass</v>
       </c>
       <c r="G43" t="str">
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
+      </c>
+      <c r="I43" t="str">
+        <v/>
       </c>
     </row>
     <row r="44">
@@ -1593,10 +1671,13 @@
         <v>Pass</v>
       </c>
       <c r="G44" t="str">
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
+      </c>
+      <c r="I44" t="str">
+        <v/>
       </c>
     </row>
     <row r="45">
@@ -1622,7 +1703,10 @@
         <v>Fail</v>
       </c>
       <c r="H45" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I45" t="str">
+        <v/>
       </c>
     </row>
     <row r="46">
@@ -1648,7 +1732,10 @@
         <v>Fail</v>
       </c>
       <c r="H46" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I46" t="str">
+        <v/>
       </c>
     </row>
     <row r="47">
@@ -1674,7 +1761,10 @@
         <v>Fail</v>
       </c>
       <c r="H47" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I47" t="str">
+        <v/>
       </c>
     </row>
     <row r="48">
@@ -1700,7 +1790,10 @@
         <v>Fail</v>
       </c>
       <c r="H48" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I48" t="str">
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -1726,7 +1819,7 @@
         <v>Fail</v>
       </c>
       <c r="H49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="str">
         <v>Login was unsuccessful</v>
@@ -1755,7 +1848,7 @@
         <v>Fail</v>
       </c>
       <c r="H50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="str">
         <v>Sorry, you have been blocked</v>
@@ -1784,7 +1877,7 @@
         <v>Fail</v>
       </c>
       <c r="H51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="str">
         <v>Login was unsuccessful</v>
@@ -1813,7 +1906,7 @@
         <v>Fail</v>
       </c>
       <c r="H52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" t="str">
         <v>Login was unsuccessful</v>
@@ -1842,7 +1935,10 @@
         <v>Fail</v>
       </c>
       <c r="H53" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I53" t="str">
+        <v/>
       </c>
     </row>
     <row r="54">
@@ -1868,7 +1964,10 @@
         <v>Fail</v>
       </c>
       <c r="H54" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I54" t="str">
+        <v/>
       </c>
     </row>
     <row r="55">
@@ -1894,7 +1993,10 @@
         <v>Fail</v>
       </c>
       <c r="H55" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I55" t="str">
+        <v/>
       </c>
     </row>
     <row r="56">
@@ -1920,7 +2022,10 @@
         <v>Fail</v>
       </c>
       <c r="H56" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I56" t="str">
+        <v/>
       </c>
     </row>
     <row r="57">
@@ -1946,7 +2051,7 @@
         <v>Fail</v>
       </c>
       <c r="H57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="str">
         <v>Login was unsuccessful</v>

</xml_diff>

<commit_message>
Modified test data and regenerated Allure test reports and attachments.
</commit_message>
<xml_diff>
--- a/test-data/loginpage1data.xlsx
+++ b/test-data/loginpage1data.xlsx
@@ -1703,7 +1703,7 @@
         <v>Fail</v>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="str">
         <v/>
@@ -1732,7 +1732,7 @@
         <v>Fail</v>
       </c>
       <c r="H46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" t="str">
         <v/>
@@ -1761,7 +1761,7 @@
         <v>Fail</v>
       </c>
       <c r="H47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="str">
         <v/>
@@ -1848,7 +1848,7 @@
         <v>Fail</v>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="str">
         <v>Sorry, you have been blocked</v>
@@ -1877,7 +1877,7 @@
         <v>Fail</v>
       </c>
       <c r="H51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="str">
         <v>Login was unsuccessful</v>
@@ -1906,7 +1906,7 @@
         <v>Fail</v>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="str">
         <v>Login was unsuccessful</v>
@@ -1935,7 +1935,7 @@
         <v>Fail</v>
       </c>
       <c r="H53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="str">
         <v/>
@@ -1964,7 +1964,7 @@
         <v>Fail</v>
       </c>
       <c r="H54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="str">
         <v/>
@@ -1993,7 +1993,7 @@
         <v>Fail</v>
       </c>
       <c r="H55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="str">
         <v/>
@@ -2022,7 +2022,7 @@
         <v>Fail</v>
       </c>
       <c r="H56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="str">
         <v/>
@@ -2051,7 +2051,7 @@
         <v>Fail</v>
       </c>
       <c r="H57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="str">
         <v>Login was unsuccessful</v>

</xml_diff>